<commit_message>
Updated to data drive the product category from the data sheet.  Additionally, found out that you have to disable smart identification on the first and second available product objects in the OR to have them properly identify by the inner text instead of by browser table location.  Lastly, added comments.
</commit_message>
<xml_diff>
--- a/Fiori_Shopping/Default.xlsx
+++ b/Fiori_Shopping/Default.xlsx
@@ -14,6 +14,20 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Laptops</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
@@ -154,7 +168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -162,13 +176,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -467,18 +497,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.4375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1"/>
+    <row customFormat="1">
+      <c t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row>
+      <c s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row>
+      <c s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated to no longer rely on R&R settings
</commit_message>
<xml_diff>
--- a/Fiori_Shopping/Default.xlsx
+++ b/Fiori_Shopping/Default.xlsx
@@ -15,15 +15,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+  <si>
+    <t>BrowserName</t>
+  </si>
+  <si>
+    <t>CHROME</t>
+  </si>
   <si>
     <t>Accessories</t>
   </si>
   <si>
+    <t>https://sapui5.hana.ondemand.com/test-resources/sap/m/demokit/cart/webapp/index.html#</t>
+  </si>
+  <si>
     <t>Categories</t>
   </si>
   <si>
     <t>Laptops</t>
+  </si>
+  <si>
+    <t>URL</t>
   </si>
 </sst>
 </file>
@@ -168,12 +180,23 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -193,12 +216,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -497,31 +523,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="1" width="10.4375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
       <c t="s">
+        <v>4</v>
+      </c>
+      <c t="s">
+        <v>0</v>
+      </c>
+      <c t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row>
+      <c s="2" t="s">
+        <v>5</v>
+      </c>
+      <c s="2" t="s">
         <v>1</v>
+      </c>
+      <c s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row>
       <c s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row>
       <c s="2" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>